<commit_message>
Additional changes. Can now paste + copy columns (although no support for copying lines, etc.) again.
</commit_message>
<xml_diff>
--- a/ColumnCopier/Assets/testInput.xlsx
+++ b/ColumnCopier/Assets/testInput.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a06cb9bda90c967/Personal Projects/ColumnCopier/ColumnCopier/Assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricky\OneDrive\Personal Projects\ColumnCopier\ColumnCopier\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>a</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>ccccc</t>
+  </si>
+  <si>
+    <t>a&lt;</t>
+  </si>
+  <si>
+    <t>bb&gt;</t>
+  </si>
+  <si>
+    <t>?4</t>
   </si>
 </sst>
 </file>
@@ -420,15 +429,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>1</v>
       </c>
@@ -438,16 +447,31 @@
       <c r="C1">
         <v>3</v>
       </c>
-      <c r="D1">
-        <v>4</v>
+      <c r="D1" t="s">
+        <v>17</v>
       </c>
       <c r="E1">
         <v>5</v>
       </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>2</v>
+      </c>
+      <c r="I1">
+        <v>3</v>
+      </c>
+      <c r="J1">
+        <v>4</v>
+      </c>
+      <c r="K1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -461,13 +485,28 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -478,8 +517,23 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -493,6 +547,21 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>